<commit_message>
added Portuguese Performance Palette (Thanks José!)
</commit_message>
<xml_diff>
--- a/mod/z02_clipit_api/libraries/performance_palette/performance_palette_de.xlsx
+++ b/mod/z02_clipit_api/libraries/performance_palette/performance_palette_de.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pebs74\Documents\PhpstormProjects\clipit_master\mod\z02_clipit_api\libraries\performance_palette\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="165"/>
   </bookViews>
@@ -407,32 +412,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <name val="Century Gothic"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Century Gothic"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="14"/>
-      <name val="Century Gothic"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="26"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Century Gothic"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -456,27 +439,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -831,7 +802,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -842,10 +813,10 @@
   <dimension ref="A1:G39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="43" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="43" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="8.5703125" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8.42578125" style="2" bestFit="1" customWidth="1"/>
@@ -858,885 +829,889 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A1" s="2" t="s">
+      <c r="A1" t="s">
         <v>30</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" t="s">
         <v>29</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" t="s">
         <v>31</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" t="s">
         <v>32</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" t="s">
         <v>33</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" t="s">
         <v>0</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A2" s="2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="C2" s="2" t="s">
+      <c r="B2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C2" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" t="s">
         <v>35</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="F2" t="s">
         <v>2</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="G2" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="18" x14ac:dyDescent="0.2">
-      <c r="A3" s="2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3">
         <v>2</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="C3" s="2" t="s">
+      <c r="B3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C3" t="s">
         <v>41</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="D3" t="s">
         <v>37</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="E3" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="F3" t="s">
         <v>2</v>
       </c>
-      <c r="G3" s="4" t="s">
+      <c r="G3" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="63.75" x14ac:dyDescent="0.2">
-      <c r="A4" s="2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4">
         <v>3</v>
       </c>
-      <c r="B4" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="C4" s="2" t="s">
+      <c r="B4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C4" t="s">
         <v>40</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="D4" t="s">
         <v>38</v>
       </c>
-      <c r="F4" s="2" t="s">
+      <c r="E4"/>
+      <c r="F4" t="s">
         <v>2</v>
       </c>
-      <c r="G4" s="4" t="s">
+      <c r="G4" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A5" s="2">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5">
         <v>4</v>
       </c>
-      <c r="B5" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="C5" s="2" t="s">
+      <c r="B5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C5" t="s">
         <v>6</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="D5" t="s">
         <v>39</v>
       </c>
-      <c r="F5" s="2" t="s">
+      <c r="E5"/>
+      <c r="F5" t="s">
         <v>2</v>
       </c>
-      <c r="G5" s="4" t="s">
+      <c r="G5" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A6" s="2">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6">
         <v>5</v>
       </c>
-      <c r="B6" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="C6" s="2" t="s">
+      <c r="B6" t="s">
+        <v>34</v>
+      </c>
+      <c r="C6" t="s">
         <v>42</v>
       </c>
-      <c r="D6" s="5" t="s">
+      <c r="D6" t="s">
         <v>43</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="E6" t="s">
         <v>7</v>
       </c>
-      <c r="F6" s="2" t="s">
+      <c r="F6" t="s">
         <v>2</v>
       </c>
-      <c r="G6" s="4" t="s">
+      <c r="G6" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="51" x14ac:dyDescent="0.2">
-      <c r="A7" s="2">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7">
         <v>6</v>
       </c>
-      <c r="B7" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="C7" s="6" t="s">
+      <c r="B7" t="s">
+        <v>34</v>
+      </c>
+      <c r="C7" t="s">
         <v>44</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="D7" t="s">
         <v>45</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="E7" t="s">
         <v>8</v>
       </c>
-      <c r="F7" s="2" t="s">
+      <c r="F7" t="s">
         <v>2</v>
       </c>
-      <c r="G7" s="4" t="s">
+      <c r="G7" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="63.75" x14ac:dyDescent="0.2">
-      <c r="A8" s="2">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8">
         <v>7</v>
       </c>
-      <c r="B8" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="C8" s="2" t="s">
+      <c r="B8" t="s">
+        <v>34</v>
+      </c>
+      <c r="C8" t="s">
         <v>46</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="D8" t="s">
         <v>47</v>
       </c>
-      <c r="E8" s="1" t="s">
+      <c r="E8" t="s">
         <v>52</v>
       </c>
-      <c r="F8" s="2" t="s">
+      <c r="F8" t="s">
         <v>2</v>
       </c>
-      <c r="G8" s="4" t="s">
+      <c r="G8" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="63.75" x14ac:dyDescent="0.2">
-      <c r="A9" s="2">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9">
         <v>8</v>
       </c>
-      <c r="B9" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="C9" s="2" t="s">
+      <c r="B9" t="s">
+        <v>34</v>
+      </c>
+      <c r="C9" t="s">
         <v>49</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="D9" t="s">
         <v>48</v>
       </c>
-      <c r="E9" s="1" t="s">
+      <c r="E9" t="s">
         <v>51</v>
       </c>
-      <c r="F9" s="2" t="s">
+      <c r="F9" t="s">
         <v>2</v>
       </c>
-      <c r="G9" s="4" t="s">
+      <c r="G9" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="51" x14ac:dyDescent="0.2">
-      <c r="A10" s="2">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10">
         <v>9</v>
       </c>
-      <c r="B10" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="C10" s="2" t="s">
+      <c r="B10" t="s">
+        <v>34</v>
+      </c>
+      <c r="C10" t="s">
         <v>9</v>
       </c>
-      <c r="D10" s="1" t="s">
+      <c r="D10" t="s">
         <v>50</v>
       </c>
-      <c r="E10" s="5"/>
-      <c r="F10" s="2" t="s">
+      <c r="E10"/>
+      <c r="F10" t="s">
         <v>2</v>
       </c>
-      <c r="G10" s="4" t="s">
+      <c r="G10" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="51" x14ac:dyDescent="0.2">
-      <c r="A11" s="2">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11">
         <v>10</v>
       </c>
-      <c r="B11" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="C11" s="2" t="s">
+      <c r="B11" t="s">
+        <v>34</v>
+      </c>
+      <c r="C11" t="s">
         <v>53</v>
       </c>
-      <c r="D11" s="5" t="s">
+      <c r="D11" t="s">
         <v>54</v>
       </c>
-      <c r="E11" s="1" t="s">
+      <c r="E11" t="s">
         <v>55</v>
       </c>
-      <c r="F11" s="2" t="s">
+      <c r="F11" t="s">
         <v>2</v>
       </c>
-      <c r="G11" s="4" t="s">
+      <c r="G11" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A12" s="2">
-        <v>11</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="C12" s="2" t="s">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>34</v>
+      </c>
+      <c r="C12" t="s">
         <v>56</v>
       </c>
-      <c r="D12" s="1" t="s">
+      <c r="D12" t="s">
         <v>57</v>
       </c>
-      <c r="E12" s="1" t="s">
+      <c r="E12" t="s">
         <v>10</v>
       </c>
-      <c r="F12" s="2" t="s">
+      <c r="F12" t="s">
         <v>2</v>
       </c>
-      <c r="G12" s="4" t="s">
+      <c r="G12" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="114.75" x14ac:dyDescent="0.2">
-      <c r="A13" s="2">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A13">
         <v>12</v>
       </c>
-      <c r="B13" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="C13" s="2" t="s">
+      <c r="B13" t="s">
+        <v>34</v>
+      </c>
+      <c r="C13" t="s">
         <v>59</v>
       </c>
-      <c r="D13" s="1" t="s">
+      <c r="D13" t="s">
         <v>58</v>
       </c>
-      <c r="F13" s="2" t="s">
+      <c r="E13"/>
+      <c r="F13" t="s">
         <v>2</v>
       </c>
-      <c r="G13" s="4" t="s">
+      <c r="G13" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="51" x14ac:dyDescent="0.2">
-      <c r="A14" s="2">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A14">
         <v>13</v>
       </c>
-      <c r="B14" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="C14" s="2" t="s">
+      <c r="B14" t="s">
+        <v>34</v>
+      </c>
+      <c r="C14" t="s">
         <v>61</v>
       </c>
-      <c r="D14" s="1" t="s">
+      <c r="D14" t="s">
         <v>60</v>
       </c>
-      <c r="E14" s="1" t="s">
+      <c r="E14" t="s">
         <v>62</v>
       </c>
-      <c r="F14" s="2" t="s">
+      <c r="F14" t="s">
         <v>2</v>
       </c>
-      <c r="G14" s="4" t="s">
+      <c r="G14" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="76.5" x14ac:dyDescent="0.2">
-      <c r="A15" s="2">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A15">
         <v>14</v>
       </c>
-      <c r="B15" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="C15" s="2" t="s">
+      <c r="B15" t="s">
+        <v>34</v>
+      </c>
+      <c r="C15" t="s">
         <v>63</v>
       </c>
-      <c r="D15" s="1" t="s">
+      <c r="D15" t="s">
         <v>64</v>
       </c>
-      <c r="F15" s="2" t="s">
+      <c r="E15"/>
+      <c r="F15" t="s">
         <v>2</v>
       </c>
-      <c r="G15" s="4" t="s">
+      <c r="G15" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="102" x14ac:dyDescent="0.2">
-      <c r="A16" s="2">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A16">
         <v>15</v>
       </c>
-      <c r="B16" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="C16" s="2" t="s">
+      <c r="B16" t="s">
+        <v>34</v>
+      </c>
+      <c r="C16" t="s">
         <v>12</v>
       </c>
-      <c r="D16" s="1" t="s">
+      <c r="D16" t="s">
         <v>66</v>
       </c>
-      <c r="E16" s="1" t="s">
+      <c r="E16" t="s">
         <v>13</v>
       </c>
-      <c r="F16" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="G16" s="1" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" ht="102" x14ac:dyDescent="0.2">
-      <c r="A17" s="2">
+      <c r="F16" t="s">
+        <v>11</v>
+      </c>
+      <c r="G16" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A17">
         <v>16</v>
       </c>
-      <c r="B17" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="C17" s="2" t="s">
+      <c r="B17" t="s">
+        <v>34</v>
+      </c>
+      <c r="C17" t="s">
         <v>67</v>
       </c>
-      <c r="D17" s="1" t="s">
+      <c r="D17" t="s">
         <v>68</v>
       </c>
-      <c r="E17" s="1" t="s">
+      <c r="E17" t="s">
         <v>69</v>
       </c>
-      <c r="F17" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="G17" s="1" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" ht="102" x14ac:dyDescent="0.2">
-      <c r="A18" s="2">
+      <c r="F17" t="s">
+        <v>11</v>
+      </c>
+      <c r="G17" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A18">
         <v>17</v>
       </c>
-      <c r="B18" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="C18" s="2" t="s">
+      <c r="B18" t="s">
+        <v>34</v>
+      </c>
+      <c r="C18" t="s">
         <v>70</v>
       </c>
-      <c r="D18" s="1" t="s">
+      <c r="D18" t="s">
         <v>71</v>
       </c>
-      <c r="E18" s="1" t="s">
+      <c r="E18" t="s">
         <v>72</v>
       </c>
-      <c r="F18" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="G18" s="1" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" ht="102" x14ac:dyDescent="0.2">
-      <c r="A19" s="2">
+      <c r="F18" t="s">
+        <v>11</v>
+      </c>
+      <c r="G18" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A19">
         <v>18</v>
       </c>
-      <c r="B19" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="C19" s="2" t="s">
+      <c r="B19" t="s">
+        <v>34</v>
+      </c>
+      <c r="C19" t="s">
         <v>73</v>
       </c>
-      <c r="D19" s="1" t="s">
+      <c r="D19" t="s">
         <v>74</v>
       </c>
-      <c r="E19" s="1" t="s">
+      <c r="E19" t="s">
         <v>14</v>
       </c>
-      <c r="F19" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="G19" s="1" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" ht="102" x14ac:dyDescent="0.2">
-      <c r="A20" s="2">
+      <c r="F19" t="s">
+        <v>11</v>
+      </c>
+      <c r="G19" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A20">
         <v>19</v>
       </c>
-      <c r="B20" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="C20" s="2" t="s">
+      <c r="B20" t="s">
+        <v>34</v>
+      </c>
+      <c r="C20" t="s">
         <v>15</v>
       </c>
-      <c r="D20" s="1" t="s">
+      <c r="D20" t="s">
         <v>75</v>
       </c>
-      <c r="E20" s="1" t="s">
+      <c r="E20" t="s">
         <v>76</v>
       </c>
-      <c r="F20" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="G20" s="1" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" ht="102" x14ac:dyDescent="0.2">
-      <c r="A21" s="2">
+      <c r="F20" t="s">
+        <v>11</v>
+      </c>
+      <c r="G20" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A21">
         <v>20</v>
       </c>
-      <c r="B21" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="C21" s="2" t="s">
+      <c r="B21" t="s">
+        <v>34</v>
+      </c>
+      <c r="C21" t="s">
         <v>16</v>
       </c>
-      <c r="D21" s="1" t="s">
+      <c r="D21" t="s">
         <v>77</v>
       </c>
-      <c r="E21" s="1" t="s">
+      <c r="E21" t="s">
         <v>78</v>
       </c>
-      <c r="F21" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="G21" s="1" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" ht="102" x14ac:dyDescent="0.2">
-      <c r="A22" s="2">
+      <c r="F21" t="s">
+        <v>11</v>
+      </c>
+      <c r="G21" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A22">
         <v>21</v>
       </c>
-      <c r="B22" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="C22" s="2" t="s">
+      <c r="B22" t="s">
+        <v>34</v>
+      </c>
+      <c r="C22" t="s">
         <v>17</v>
       </c>
-      <c r="D22" s="1" t="s">
+      <c r="D22" t="s">
         <v>79</v>
       </c>
-      <c r="E22" s="1" t="s">
+      <c r="E22" t="s">
         <v>80</v>
       </c>
-      <c r="F22" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="G22" s="1" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" ht="102" x14ac:dyDescent="0.2">
-      <c r="A23" s="2">
+      <c r="F22" t="s">
+        <v>11</v>
+      </c>
+      <c r="G22" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A23">
         <v>22</v>
       </c>
-      <c r="B23" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="C23" s="2" t="s">
+      <c r="B23" t="s">
+        <v>34</v>
+      </c>
+      <c r="C23" t="s">
         <v>18</v>
       </c>
-      <c r="D23" s="1" t="s">
+      <c r="D23" t="s">
         <v>81</v>
       </c>
-      <c r="E23" s="1" t="s">
+      <c r="E23" t="s">
         <v>19</v>
       </c>
-      <c r="F23" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="G23" s="1" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" ht="102" x14ac:dyDescent="0.2">
-      <c r="A24" s="2">
+      <c r="F23" t="s">
+        <v>11</v>
+      </c>
+      <c r="G23" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A24">
         <v>23</v>
       </c>
-      <c r="B24" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="C24" s="2" t="s">
+      <c r="B24" t="s">
+        <v>34</v>
+      </c>
+      <c r="C24" t="s">
         <v>20</v>
       </c>
-      <c r="D24" s="1" t="s">
+      <c r="D24" t="s">
         <v>82</v>
       </c>
-      <c r="E24" s="1" t="s">
+      <c r="E24" t="s">
         <v>83</v>
       </c>
-      <c r="F24" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="G24" s="1" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" ht="102" x14ac:dyDescent="0.2">
-      <c r="A25" s="2">
+      <c r="F24" t="s">
+        <v>11</v>
+      </c>
+      <c r="G24" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A25">
         <v>24</v>
       </c>
-      <c r="B25" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="C25" s="2" t="s">
+      <c r="B25" t="s">
+        <v>34</v>
+      </c>
+      <c r="C25" t="s">
         <v>84</v>
       </c>
-      <c r="D25" s="1" t="s">
+      <c r="D25" t="s">
         <v>85</v>
       </c>
-      <c r="E25" s="1" t="s">
+      <c r="E25" t="s">
         <v>21</v>
       </c>
-      <c r="F25" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="G25" s="1" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" ht="102" x14ac:dyDescent="0.2">
-      <c r="A26" s="2">
+      <c r="F25" t="s">
+        <v>11</v>
+      </c>
+      <c r="G25" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A26">
         <v>25</v>
       </c>
-      <c r="B26" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="C26" s="2" t="s">
+      <c r="B26" t="s">
+        <v>34</v>
+      </c>
+      <c r="C26" t="s">
         <v>22</v>
       </c>
-      <c r="D26" s="1" t="s">
+      <c r="D26" t="s">
         <v>86</v>
       </c>
-      <c r="E26" s="1" t="s">
+      <c r="E26" t="s">
         <v>87</v>
       </c>
-      <c r="F26" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="G26" s="1" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" ht="102" x14ac:dyDescent="0.2">
-      <c r="A27" s="2">
+      <c r="F26" t="s">
+        <v>11</v>
+      </c>
+      <c r="G26" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A27">
         <v>26</v>
       </c>
-      <c r="B27" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="C27" s="2" t="s">
+      <c r="B27" t="s">
+        <v>34</v>
+      </c>
+      <c r="C27" t="s">
         <v>88</v>
       </c>
-      <c r="D27" s="1" t="s">
+      <c r="D27" t="s">
         <v>89</v>
       </c>
-      <c r="E27" s="1" t="s">
+      <c r="E27" t="s">
         <v>90</v>
       </c>
-      <c r="F27" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="G27" s="1" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" ht="102" x14ac:dyDescent="0.2">
-      <c r="A28" s="2">
+      <c r="F27" t="s">
+        <v>11</v>
+      </c>
+      <c r="G27" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A28">
         <v>27</v>
       </c>
-      <c r="B28" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="C28" s="2" t="s">
+      <c r="B28" t="s">
+        <v>34</v>
+      </c>
+      <c r="C28" t="s">
         <v>91</v>
       </c>
-      <c r="D28" s="1" t="s">
+      <c r="D28" t="s">
         <v>92</v>
       </c>
-      <c r="E28" s="1" t="s">
+      <c r="E28" t="s">
         <v>93</v>
       </c>
-      <c r="F28" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="G28" s="1" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" ht="102" x14ac:dyDescent="0.2">
-      <c r="A29" s="2">
+      <c r="F28" t="s">
+        <v>11</v>
+      </c>
+      <c r="G28" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A29">
         <v>28</v>
       </c>
-      <c r="B29" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="C29" s="2" t="s">
+      <c r="B29" t="s">
+        <v>34</v>
+      </c>
+      <c r="C29" t="s">
         <v>23</v>
       </c>
-      <c r="D29" s="1" t="s">
+      <c r="D29" t="s">
         <v>94</v>
       </c>
-      <c r="E29" s="1" t="s">
+      <c r="E29" t="s">
         <v>95</v>
       </c>
-      <c r="F29" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="G29" s="1" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" ht="102" x14ac:dyDescent="0.2">
-      <c r="A30" s="2">
+      <c r="F29" t="s">
+        <v>11</v>
+      </c>
+      <c r="G29" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A30">
         <v>29</v>
       </c>
-      <c r="B30" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="C30" s="2" t="s">
+      <c r="B30" t="s">
+        <v>34</v>
+      </c>
+      <c r="C30" t="s">
         <v>59</v>
       </c>
-      <c r="D30" s="1" t="s">
+      <c r="D30" t="s">
         <v>107</v>
       </c>
-      <c r="E30" s="1" t="s">
+      <c r="E30" t="s">
         <v>108</v>
       </c>
-      <c r="F30" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="G30" s="1" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" ht="102" x14ac:dyDescent="0.2">
-      <c r="A31" s="2">
+      <c r="F30" t="s">
+        <v>11</v>
+      </c>
+      <c r="G30" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A31">
         <v>30</v>
       </c>
-      <c r="B31" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="C31" s="2" t="s">
+      <c r="B31" t="s">
+        <v>34</v>
+      </c>
+      <c r="C31" t="s">
         <v>104</v>
       </c>
-      <c r="D31" s="1" t="s">
+      <c r="D31" t="s">
         <v>105</v>
       </c>
-      <c r="E31" s="1" t="s">
+      <c r="E31" t="s">
         <v>106</v>
       </c>
-      <c r="F31" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="G31" s="1" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" ht="102" x14ac:dyDescent="0.2">
-      <c r="A32" s="2">
+      <c r="F31" t="s">
+        <v>11</v>
+      </c>
+      <c r="G31" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A32">
         <v>31</v>
       </c>
-      <c r="B32" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="C32" s="2" t="s">
+      <c r="B32" t="s">
+        <v>34</v>
+      </c>
+      <c r="C32" t="s">
         <v>42</v>
       </c>
-      <c r="D32" s="1" t="s">
+      <c r="D32" t="s">
         <v>103</v>
       </c>
-      <c r="E32" s="1" t="s">
+      <c r="E32" t="s">
         <v>24</v>
       </c>
-      <c r="F32" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="G32" s="1" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" ht="102" x14ac:dyDescent="0.2">
-      <c r="A33" s="2">
+      <c r="F32" t="s">
+        <v>11</v>
+      </c>
+      <c r="G32" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A33">
         <v>32</v>
       </c>
-      <c r="B33" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="C33" s="2" t="s">
+      <c r="B33" t="s">
+        <v>34</v>
+      </c>
+      <c r="C33" t="s">
         <v>25</v>
       </c>
-      <c r="D33" s="1" t="s">
+      <c r="D33" t="s">
         <v>101</v>
       </c>
-      <c r="E33" s="1" t="s">
+      <c r="E33" t="s">
         <v>102</v>
       </c>
-      <c r="F33" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="G33" s="1" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" ht="102" x14ac:dyDescent="0.2">
-      <c r="A34" s="2">
+      <c r="F33" t="s">
+        <v>11</v>
+      </c>
+      <c r="G33" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A34">
         <v>33</v>
       </c>
-      <c r="B34" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="C34" s="2" t="s">
+      <c r="B34" t="s">
+        <v>34</v>
+      </c>
+      <c r="C34" t="s">
         <v>98</v>
       </c>
-      <c r="D34" s="1" t="s">
+      <c r="D34" t="s">
         <v>99</v>
       </c>
-      <c r="E34" s="1" t="s">
+      <c r="E34" t="s">
         <v>100</v>
       </c>
-      <c r="F34" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="G34" s="1" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" ht="102" x14ac:dyDescent="0.2">
-      <c r="A35" s="2">
-        <v>34</v>
-      </c>
-      <c r="B35" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="C35" s="2" t="s">
+      <c r="F34" t="s">
+        <v>11</v>
+      </c>
+      <c r="G34" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A35">
+        <v>34</v>
+      </c>
+      <c r="B35" t="s">
+        <v>34</v>
+      </c>
+      <c r="C35" t="s">
         <v>96</v>
       </c>
-      <c r="D35" s="1" t="s">
+      <c r="D35" t="s">
         <v>97</v>
       </c>
-      <c r="E35" s="1" t="s">
+      <c r="E35" t="s">
         <v>26</v>
       </c>
-      <c r="F35" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="G35" s="1" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" ht="76.5" x14ac:dyDescent="0.2">
-      <c r="A36" s="2">
+      <c r="F35" t="s">
+        <v>11</v>
+      </c>
+      <c r="G35" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A36">
         <v>35</v>
       </c>
-      <c r="B36" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="C36" s="2" t="s">
+      <c r="B36" t="s">
+        <v>34</v>
+      </c>
+      <c r="C36" t="s">
         <v>28</v>
       </c>
-      <c r="D36" s="1" t="s">
+      <c r="D36" t="s">
         <v>110</v>
       </c>
-      <c r="E36" s="1" t="s">
+      <c r="E36" t="s">
         <v>111</v>
       </c>
-      <c r="F36" s="2" t="s">
+      <c r="F36" t="s">
         <v>27</v>
       </c>
-      <c r="G36" s="4" t="s">
+      <c r="G36" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="37" spans="1:7" ht="63.75" x14ac:dyDescent="0.2">
-      <c r="A37" s="2">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A37">
         <v>36</v>
       </c>
-      <c r="B37" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="C37" s="2" t="s">
+      <c r="B37" t="s">
+        <v>34</v>
+      </c>
+      <c r="C37" t="s">
         <v>113</v>
       </c>
-      <c r="D37" s="1" t="s">
+      <c r="D37" t="s">
         <v>112</v>
       </c>
-      <c r="E37" s="1" t="s">
+      <c r="E37" t="s">
         <v>114</v>
       </c>
-      <c r="F37" s="2" t="s">
+      <c r="F37" t="s">
         <v>27</v>
       </c>
-      <c r="G37" s="4" t="s">
+      <c r="G37" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="38" spans="1:7" ht="76.5" x14ac:dyDescent="0.2">
-      <c r="A38" s="2">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A38">
         <v>37</v>
       </c>
-      <c r="B38" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="C38" s="2" t="s">
+      <c r="B38" t="s">
+        <v>34</v>
+      </c>
+      <c r="C38" t="s">
         <v>115</v>
       </c>
-      <c r="D38" s="1" t="s">
+      <c r="D38" t="s">
         <v>116</v>
       </c>
-      <c r="E38" s="1" t="s">
+      <c r="E38" t="s">
         <v>117</v>
       </c>
-      <c r="F38" s="2" t="s">
+      <c r="F38" t="s">
         <v>27</v>
       </c>
-      <c r="G38" s="4" t="s">
+      <c r="G38" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="39" spans="1:7" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A39" s="2">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A39">
         <v>38</v>
       </c>
-      <c r="B39" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="C39" s="2" t="s">
+      <c r="B39" t="s">
+        <v>34</v>
+      </c>
+      <c r="C39" t="s">
         <v>119</v>
       </c>
-      <c r="D39" s="1" t="s">
+      <c r="D39" t="s">
         <v>118</v>
       </c>
-      <c r="E39" s="1" t="s">
+      <c r="E39" t="s">
         <v>120</v>
       </c>
-      <c r="F39" s="2" t="s">
+      <c r="F39" t="s">
         <v>27</v>
       </c>
-      <c r="G39" s="4" t="s">
+      <c r="G39" t="s">
         <v>109</v>
       </c>
     </row>

</xml_diff>